<commit_message>
SPECIFIS OLD COLD IN 12S
</commit_message>
<xml_diff>
--- a/WADE003-arcticpred_dada2_QAQC_12SP1_output-addspecies-2.xlsx
+++ b/WADE003-arcticpred_dada2_QAQC_12SP1_output-addspecies-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_A2E39DCA8F79A8D366075C52F37BD2724AC34C75" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF94658-B8B1-4320-A39B-C8B1643CCE33}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_A2E39DCA8F79A8D366075C52F37BD2724AC34C75" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18EC44C6-E686-4D7F-896E-174F59764D25}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="312">
   <si>
     <t>rownames</t>
   </si>
@@ -954,6 +954,9 @@
   </si>
   <si>
     <t>TATACGAGAGGCCCAAGTTGACAAACAACGGCGTAAAGAGTGGTTAGGGGATTTACTAAACTAGAGCCGAACGCTTTCAAAGCTGTTATACGCACCCGAAAGTATGAAACCCACGAAAGCTAAG</t>
+  </si>
+  <si>
+    <t>Species.1</t>
   </si>
 </sst>
 </file>
@@ -5637,8 +5640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773EA8D4-0049-40E7-85D0-1914524C9255}">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5649,6 +5652,8 @@
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5677,7 +5682,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>